<commit_message>
ali current courses added
</commit_message>
<xml_diff>
--- a/Data/student/Ali.xlsx
+++ b/Data/student/Ali.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zain4\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Batool\sen project\SeniorProject\Data\student\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9FB3E7-F065-49D4-BDF7-0E1394A038C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD14A00-1E49-4383-9041-E058CFABDDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="92">
   <si>
     <t>student_id</t>
   </si>
@@ -269,13 +269,40 @@
   </si>
   <si>
     <t>FREN 141</t>
+  </si>
+  <si>
+    <t>HRLC107</t>
+  </si>
+  <si>
+    <t>First 2024-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITCY401 </t>
+  </si>
+  <si>
+    <t>ITCY470</t>
+  </si>
+  <si>
+    <t>ITCY480</t>
+  </si>
+  <si>
+    <t>Human Rights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information Security </t>
+  </si>
+  <si>
+    <t>IT Auditing and Business Continuity</t>
+  </si>
+  <si>
+    <t>Cyberethics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +314,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,12 +360,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -639,27 +675,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScale="74" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="16.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="23.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="37.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="2"/>
+    <col min="6" max="6" width="16.54296875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,7 +725,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>202108899</v>
       </c>
@@ -715,7 +751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>202108899</v>
       </c>
@@ -741,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>202108899</v>
       </c>
@@ -767,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>202108899</v>
       </c>
@@ -793,7 +829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>202108899</v>
       </c>
@@ -819,7 +855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>202108899</v>
       </c>
@@ -845,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>202108899</v>
       </c>
@@ -871,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>202108899</v>
       </c>
@@ -897,7 +933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>202108899</v>
       </c>
@@ -923,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>202108899</v>
       </c>
@@ -949,7 +985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>202108899</v>
       </c>
@@ -975,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>202108899</v>
       </c>
@@ -1001,7 +1037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>202108899</v>
       </c>
@@ -1027,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>202108899</v>
       </c>
@@ -1053,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>202108899</v>
       </c>
@@ -1079,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>202108899</v>
       </c>
@@ -1108,7 +1144,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>202108899</v>
       </c>
@@ -1134,7 +1170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>202108899</v>
       </c>
@@ -1160,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>202108899</v>
       </c>
@@ -1186,7 +1222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>202108899</v>
       </c>
@@ -1212,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>202108899</v>
       </c>
@@ -1238,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>202108899</v>
       </c>
@@ -1264,7 +1300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>202108899</v>
       </c>
@@ -1290,7 +1326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>202108899</v>
       </c>
@@ -1316,7 +1352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>202108899</v>
       </c>
@@ -1342,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>202108899</v>
       </c>
@@ -1368,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>202108899</v>
       </c>
@@ -1394,7 +1430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>202108899</v>
       </c>
@@ -1420,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>202108899</v>
       </c>
@@ -1446,7 +1482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>202108899</v>
       </c>
@@ -1472,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>202108899</v>
       </c>
@@ -1498,7 +1534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>202108899</v>
       </c>
@@ -1524,7 +1560,144 @@
         <v>1</v>
       </c>
     </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>202108899</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2</v>
+      </c>
+      <c r="G34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>202108899</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="2">
+        <v>3</v>
+      </c>
+      <c r="G35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>202108899</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" s="2">
+        <v>3</v>
+      </c>
+      <c r="G36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>202108899</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E37" s="2">
+        <v>3</v>
+      </c>
+      <c r="G37" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>202108899</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="2">
+        <v>3</v>
+      </c>
+      <c r="G38" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>202108899</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="2">
+        <v>3</v>
+      </c>
+      <c r="G39" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>